<commit_message>
Version - solucionar bugs
</commit_message>
<xml_diff>
--- a/info_excel.xlsx
+++ b/info_excel.xlsx
@@ -7,7 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BCP SOLES" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BCP DOLARES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="BBVA SOLES" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BBVA DOLARES" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SCOTIA SOLES" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SCOTIA DOLARES" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,13 +430,29 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -441,247 +462,1313 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Comprobante</t>
+          <t>Fecha valuta</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>Descripcion operacion</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Estado</t>
+          <t>Monto</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Saldo</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sucursal-Agencia</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Operacion numero</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Operacion hora</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Guias</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Moneda</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Monto de la factura</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Monto (S/)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-08-24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>FP01-0001</t>
+          <t>09/01/2022</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>INVERSIONES MIJEY E.I.R.L.</t>
+          <t>IMPUESTO ITF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Generada</t>
+          <t>-0.15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>USR-2</t>
+          <t>25659.92</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['T001-1000', 'T001-1001']</t>
+          <t>000-000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SOLES</t>
+          <t>0      0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>454.40</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>454.40</t>
+          <t>BATCH</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0909  </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-08-30</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>FP01-0002</t>
+          <t>09/01/2022</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>REDES Y APAREJOS DEL MAR S.A.C.</t>
+          <t>A 310 04583620 0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Generada</t>
+          <t>-1480.24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>USR-3</t>
+          <t>25660.07</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>111-008</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>SOLES</t>
+          <t>02018319</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3594.25</t>
+          <t>10:34:33</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3594.25</t>
+          <t>TNP0WH</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-09-11</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FP01-0003</t>
+          <t>09/01/2022</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GM INGENIEROS NACIONALES S.A.C</t>
+          <t>TELE 913339240</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Generada</t>
+          <t>-59.9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>USR-4</t>
+          <t>27140.31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>111-008</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>DOLARES</t>
+          <t>00013439</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1106.10</t>
+          <t>10:00:39</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>4294.50</t>
+          <t>TNP0O3</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4404  </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-09-11</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>FP01-0004</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>09/01/2022</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ENTR.EFEC. 0178727</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Generada</t>
+          <t>2138.86</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>USR-3</t>
+          <t>27200.21</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>310-000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>DOLARES</t>
+          <t>00178727</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>359.76</t>
+          <t>17:36:13</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1384.08</t>
+          <t>T19357</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1018  </t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>IMPUESTO ITF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-1.35</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>634.98</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>000-000</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Monto Total</t>
+          <t>0      0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5514.51</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>BATCH</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0909  </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A 570 91973463 0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-25000.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>636.33</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>02011898</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>09:58:46</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>TNP0KA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A 570 91973463 0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-1931.8</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>25636.33</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>02032896</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>11:58:34</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>TNP0DQ</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>A 310 04583620 0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-1491.6</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>27568.13</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>02064079</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>16:23:29</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>TNP379</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>TELE 913339240</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-59.9</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>29059.73</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>05034297</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>12:36:21</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>TNP0KS</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4404  </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>DE METALPROTEC S.A.C.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>26992.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>29119.63</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>02010631</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>09:48:28</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>TNP0LW</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2406  </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TRAN.CTAS.TERC.BM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>566.76</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2127.63</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>111-023</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>00259871</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>11:06:07</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>BMO992</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2701  </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha valuta</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Descripcion operacion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Monto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Saldo</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sucursal-Agencia</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Operacion numero</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Operacion hora</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Vendedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>09/01/2022</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>IMPUESTO ITF</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-0.2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4877.54</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>000-000</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0      0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>BATCH</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0909  </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09/01/2022</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A 193 1165447 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-4786.61</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4877.74</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>02084511</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>17:34:34</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>TNP0SG</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>09/01/2022</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TRAN.CTAS.TERC.BM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>142.85</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>9664.35</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>111-023</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>01324575</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>14:31:08</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>BMO250</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2701  </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IMPUESTO ITF</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-0.7</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>8898.88</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>000-000</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0      0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>BATCH</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0909  </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A 193 1165447 1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-14202.34</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>8899.58</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>02061844</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>16:10:26</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>TNP027</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4401  </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>08/01/2022</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A 310 9888337 0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-7000.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>23101.92</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>111-008</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>01010631</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>09:48:28</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>TNP0LW</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4406  </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F.Operacion</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>F.Valor</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Referencia</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Importe</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ITF</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Num.Mvto</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Vendedor</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F.Operacion</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>F.Valor</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Referencia</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Importe</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ITF</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Num.Mvto</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Vendedor</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCION</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Nro.DOC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CARGO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ABONO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Vendedor</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DESCRIPCION</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Nro.DOC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CARGO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ABONO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cotizacion</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Guia</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>F/B</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Vendedor</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[ADD] Kits de productos implementados
</commit_message>
<xml_diff>
--- a/info_excel.xlsx
+++ b/info_excel.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,13 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,156 +481,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="n">
-        <v>44808</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ingreso</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Trujillo</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>44808</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ingreso</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chiclayo</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>44857</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Ingreso</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lima</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>55.0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>90.0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Traslado</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Lima</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>90.0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>90.0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>44927</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Traslado</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Chimbote</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>90.0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>90.0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] Cambio en comisiones
</commit_message>
<xml_diff>
--- a/info_excel.xlsx
+++ b/info_excel.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,11 +441,6 @@
     <col width="30" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="30" customWidth="1" min="6" max="6"/>
-    <col width="30" customWidth="1" min="7" max="7"/>
-    <col width="30" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,32 +451,446 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Referencia</t>
+          <t>Codigo</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Almacen</t>
+          <t>Cliente</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Stock anterior</t>
+          <t>Nro operacion</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Nuevo Stock</t>
+          <t>Nro operacion 2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Cantidad de ingreso</t>
+          <t>Moneda</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Cantidad de egreso</t>
+          <t>Monto sin IGV</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>44928</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>F001-0298</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PESQUERA CONCEPCION S.A.C.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2867.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>44928</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>F001-0299</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MEGUI INVESTMENT S.A.C.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>171693</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>412.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>F001-0300</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EMPRESA GRUPO JIVO SOCIEDAD ANONIMA CERRADA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1273480</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1658.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>F001-0304</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OROSCO CASTRO JIMMY NICOLAY</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>69082</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>390.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>F001-0305</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>EMPRESA PESQUERA ROSA ISABEL S.R.L.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1830879</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2191.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>F001-0306</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OROSCO CASTRO JIMMY NICOLAY</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1986175</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>68.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>F001-0307</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>STEEL ASESORIA E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>243534597</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>146.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>F001-0308</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>STEEL ASESORIA E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>243536416</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>213.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>F001-0309</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MEGUI INVESTMENT S.A.C.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>39411</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>4149.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>F001-0311</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>EMPRESA PESQUERA ROSA ISABEL S.R.L.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1146102</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>429.74</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>F001-0312</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AITANA&amp;KHALEESI E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>DOLARES</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>3186.72</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>F001-0313</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SERVICIOS INDUSTRIALES HALAVISI S.A.C.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1785131</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>178.29</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>F001-0314</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SERVICIOS INDUSTRIALES HALAVISI S.A.C.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1756488</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>73.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Monto total</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>15966.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Monto comision</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>159.66</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD]Funcion para importar registro de costos
</commit_message>
<xml_diff>
--- a/info_excel.xlsx
+++ b/info_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,17 +433,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="40" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -459,161 +457,368 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>Cliente / (Producto / Servicio)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RUC</t>
+          <t>Estado</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Estado</t>
+          <t>Vendedor</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Vendedor</t>
+          <t>Guias</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Guias</t>
+          <t>Moneda</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Item</t>
+          <t>Monto de la boleta</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Moneda</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>PU (SIN IGV) S/</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Cantidad</t>
+          <t>Monto (S/)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-04-10</t>
+          <t>2023-04-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B001-0023</t>
+          <t>B001-0028</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SEGUNDO CARCAMO NIZAMA</t>
+          <t>MARIA LUZ PEREZ DE RAMOS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>32804324</t>
+          <t>Aceptado</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Aceptado</t>
+          <t>USR-16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>USR-16</t>
+          <t>['T001-0617']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['T001-0573']</t>
+          <t>SOLES</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FASTIMAS MASILLA - PARTE A . 1/2 GL</t>
+          <t>512.18</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>SOLES</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>69.52</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>512.18</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B001-0027</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">METALPROTEC S.A.C </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>USR-16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['T001-0613']</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1042.15</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1042.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B001-0026</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">METALPROTEC S.A.C </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>USR-16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['T001-0611']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>733.46</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>733.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-04-24</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B001-0025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ELIAS MARCHENA MARCHENA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Aceptado</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>USR-16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['T001-0603']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>258.21</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>258.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-04-19</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B001-0024</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ELIAS MARCHENA MARCHENA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Aceptado</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>USR-16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['T001-0593']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>259.11</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>259.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>2023-04-10</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>B001-0023</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>SEGUNDO CARCAMO NIZAMA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>32804324</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Aceptado</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>USR-16</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>['T001-0573']</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>FASTIMAS MASILLA - PARTE B . 1/2 GL</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>SOLES</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>69.52</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>139.04</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>139.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-04-01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B001-0022</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>EUSTACIO VIDAL CESPEDES</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Aceptado</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>USR-16</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['T001-0561']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>154.77</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>154.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Monto Total</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1323.31</t>
         </is>
       </c>
     </row>

</xml_diff>